<commit_message>
bug fixes 1. opening whatsapp if not opened 2. replacing reserved URL characters
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\python\WhatsAppMesgAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F9C71B-B6AD-44A5-845F-BE80B725A77E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D564E53-29FF-4E1A-B113-1BA9634B5097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>mobile number</t>
   </si>
@@ -35,25 +35,21 @@
   <si>
     <t>image</t>
   </si>
-  <si>
-    <t>one</t>
-  </si>
-  <si>
-    <t>two</t>
-  </si>
-  <si>
-    <t>one.png</t>
-  </si>
-  <si>
-    <t>two.jpg</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -69,7 +65,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -77,12 +73,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -364,50 +376,28 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.109375" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="33.21875" customWidth="1"/>
     <col min="3" max="3" width="29.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>88914154571425</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>8891415457</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added country code in the contacts.xlsx file
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\python\WhatsAppMesgAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D564E53-29FF-4E1A-B113-1BA9634B5097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6F6707-3B56-4A48-BF1C-D7459B29C2FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>mobile number</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>image</t>
+  </si>
+  <si>
+    <t>country code</t>
   </si>
 </sst>
 </file>
@@ -50,19 +53,25 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -94,7 +103,9 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,10 +387,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -387,16 +398,20 @@
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="33.21875" customWidth="1"/>
     <col min="3" max="3" width="29.5546875" customWidth="1"/>
+    <col min="4" max="4" width="35.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>